<commit_message>
Added the extent report and send mails classes
</commit_message>
<xml_diff>
--- a/target/classes/com/testdata/TestSuite1.xlsx
+++ b/target/classes/com/testdata/TestSuite1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="44">
   <si>
     <t>TCID</t>
   </si>
@@ -133,6 +133,21 @@
   </si>
   <si>
     <t>Search and selecting the designation text box.</t>
+  </si>
+  <si>
+    <t>TC_002_Validate_NearBy_Homes_page</t>
+  </si>
+  <si>
+    <t>Validate the near by homes page count</t>
+  </si>
+  <si>
+    <t>scroll_Down</t>
+  </si>
+  <si>
+    <t>nearyoutext</t>
+  </si>
+  <si>
+    <t>NearBy homes location selector</t>
   </si>
 </sst>
 </file>
@@ -526,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,6 +576,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -568,10 +594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,6 +801,78 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>